<commit_message>
Updated Turks for costs and climate
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/total_costs.xlsx
+++ b/scripts/query_generator/cost_update/total_costs.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="backup" sheetId="2" r:id="rId2"/>
+    <sheet name="20121221" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="backup" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20121221'!$A$1:$B$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$131</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="160">
   <si>
     <t>key</t>
   </si>
@@ -476,6 +478,33 @@
   </si>
   <si>
     <t>EXCEL_TABLE(G(cost_other),</t>
+  </si>
+  <si>
+    <t>nergy_chp_ultra_supercritical_coal</t>
+  </si>
+  <si>
+    <t>agriculture_chp_engine_natural_gas</t>
+  </si>
+  <si>
+    <t>buildings_collective_chp_natural_gas</t>
+  </si>
+  <si>
+    <t>energy_chp_combined_cycle_network_gas</t>
+  </si>
+  <si>
+    <t>energy_power_combined_cycle_ccs_network_gas</t>
+  </si>
+  <si>
+    <t>energy_power_combined_cycle_network_gas</t>
+  </si>
+  <si>
+    <t>energy_power_ultra_supercritical_network_gas</t>
+  </si>
+  <si>
+    <t>other_chp_engine_network_gas</t>
+  </si>
+  <si>
+    <t>energy_heat_network_backup_heater_network_gas</t>
   </si>
 </sst>
 </file>
@@ -529,8 +558,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -538,9 +571,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,10 +907,967 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B116"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="87.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>669753.66372214095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>369782.98504606402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>518989.66055762197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5">
+        <v>451954.62750842603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16">
+      <c r="A8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8">
+        <v>232359.57840255499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>62923335.085405901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16">
+      <c r="A10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16">
+      <c r="A11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16">
+      <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16">
+      <c r="A13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13">
+        <v>858888.40538922697</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>587333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>2545.2924119999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>4942.5355584795898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16">
+      <c r="A17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18">
+        <v>9715.0614771573091</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20">
+        <v>195.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21">
+        <v>618052.75086526002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>2507.69425586742</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16">
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>13386.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16">
+      <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <v>9643.7388078544791</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16">
+      <c r="A25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25">
+        <v>251658655.71277899</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>250935350.003824</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>377260702.42225301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>135687530.408627</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>84195425.480663896</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16">
+      <c r="A30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31">
+        <v>5202804.4875486996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32">
+        <v>14596149.849582899</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16">
+      <c r="A33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16">
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16">
+      <c r="A35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35">
+        <v>8821748.2849042695</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16">
+      <c r="A36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16">
+      <c r="A37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37">
+        <v>9879467.9617414791</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>282404665.385589</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16">
+      <c r="A39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39">
+        <v>267656871.20731199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16">
+      <c r="A40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>244612695.44406801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16">
+      <c r="A41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41">
+        <v>265687203.37454599</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16">
+      <c r="A42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42">
+        <v>327951301.000947</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43">
+        <v>9315783.8983050808</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16">
+      <c r="A44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16">
+      <c r="A45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45">
+        <v>56067143.149989001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16">
+      <c r="A46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16">
+      <c r="A47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16">
+      <c r="A48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16">
+      <c r="A49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16">
+      <c r="A50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>366156088.48758399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16">
+      <c r="A51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>647123302.82240796</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16">
+      <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52">
+        <v>15154166.3333333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16">
+      <c r="A53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53">
+        <v>4236515.3599999901</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>178126907.15206799</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16">
+      <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55">
+        <v>27279530.952380899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16">
+      <c r="A56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16">
+      <c r="A57" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16">
+      <c r="A58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58">
+        <v>17705160.810299501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16">
+      <c r="A59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>262124830.59272301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16">
+      <c r="A60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>262363802.82582599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16">
+      <c r="A61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61">
+        <v>512651919.961757</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="16">
+      <c r="A62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62">
+        <v>327951301.000947</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="16">
+      <c r="A63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>181196389.517434</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="16">
+      <c r="A64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64">
+        <v>106339848.537673</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="16">
+      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65">
+        <v>315233432.18682897</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="16">
+      <c r="A66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="16">
+      <c r="A67" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="16">
+      <c r="A68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="16">
+      <c r="A69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69">
+        <v>266816.53177964699</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="16">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>60587576.139797598</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="16">
+      <c r="A71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="16">
+      <c r="A72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="16">
+      <c r="A73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="16">
+      <c r="A74" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="16">
+      <c r="A75" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="16">
+      <c r="A76" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76">
+        <v>222.92452080000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16">
+      <c r="A77" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77">
+        <v>358.654464235619</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="16">
+      <c r="A78" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B78">
+        <v>513.729031978796</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="16">
+      <c r="A79" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79">
+        <v>845.19104734837197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="16">
+      <c r="A80" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16">
+      <c r="A81" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16">
+      <c r="A82" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16">
+      <c r="A83" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16">
+      <c r="A84" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16">
+      <c r="A85" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="16">
+      <c r="A86" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86">
+        <v>578.09109640171903</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="16">
+      <c r="A87" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B87">
+        <v>802.50077049713502</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="16">
+      <c r="A88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16">
+      <c r="A89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89">
+        <v>322.87188184190501</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16">
+      <c r="A90" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="16">
+      <c r="A91" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16">
+      <c r="A92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="16">
+      <c r="A93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16">
+      <c r="A94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16">
+      <c r="A95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16">
+      <c r="A96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B96">
+        <v>199.11984128017099</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16">
+      <c r="A97" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B97">
+        <v>14.68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16">
+      <c r="A98" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B98">
+        <v>94.78</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16">
+      <c r="A99" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99">
+        <v>476.61081081081102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16">
+      <c r="A100" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B100">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16">
+      <c r="A101" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101">
+        <v>4926635.1499049403</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16">
+      <c r="A102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B102">
+        <v>12767744.447830999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16">
+      <c r="A103" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B103">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16">
+      <c r="A104" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B104">
+        <v>9991043.3145009391</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16">
+      <c r="A105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105">
+        <v>18731502.137926701</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16">
+      <c r="A106" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106">
+        <v>33013074.907786202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16">
+      <c r="A107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107">
+        <v>6447245.6891400497</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="16">
+      <c r="A108" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B108">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="16">
+      <c r="A109" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109">
+        <v>4478766.8760734303</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="16">
+      <c r="A110" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B110">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="16">
+      <c r="A111" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B111">
+        <v>250935350.003824</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="16">
+      <c r="A112" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112">
+        <v>4926635.1499049403</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="16">
+      <c r="A113" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B113">
+        <v>669753.66372214095</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="16">
+      <c r="A114" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114">
+        <v>369782.98504606402</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="16">
+      <c r="A115" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B115">
+        <v>518989.66055762197</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="16">
+      <c r="A116" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B116">
+        <v>209718.165600915</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B116">
+    <sortState ref="A2:B131">
+      <sortCondition ref="A1:A131"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B131"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1946,7 +2940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F156"/>
   <sheetViews>
@@ -3184,6 +4178,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fixed costs to correspond to CHP cleanup.
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/total_costs.xlsx
+++ b/scripts/query_generator/cost_update/total_costs.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="20121221" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="backup" sheetId="2" r:id="rId3"/>
+    <sheet name="20130409" sheetId="4" r:id="rId1"/>
+    <sheet name="20121221" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="backup" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20121221'!$A$1:$B$116</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'20121221'!$A$1:$B$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20130409'!$A$1:$B$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$B$131</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="164">
   <si>
     <t>key</t>
   </si>
@@ -505,6 +507,18 @@
   </si>
   <si>
     <t>energy_heat_network_backup_heater_network_gas</t>
+  </si>
+  <si>
+    <t>agriculture_chp_engine_biogas</t>
+  </si>
+  <si>
+    <t>agriculture_chp_engine_network_gas</t>
+  </si>
+  <si>
+    <t>industry_chp_engine_gas_power_fuelmix</t>
+  </si>
+  <si>
+    <t>industry_chp_turbine_gas_power_fuelmix</t>
   </si>
 </sst>
 </file>
@@ -558,8 +572,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -571,13 +591,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -907,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:XFD71"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -953,503 +979,503 @@
     </row>
     <row r="5" spans="1:2" ht="16">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B5">
-        <v>451954.62750842603</v>
+        <v>701111.13218570501</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="B6">
-        <v>793333.33333333302</v>
+        <v>712226.358094853</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7">
-        <v>404644.32235354203</v>
+        <v>793333.33333333302</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="B8">
-        <v>232359.57840255499</v>
+        <v>404644.32235354203</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>153</v>
       </c>
       <c r="B9">
-        <v>62923335.085405901</v>
+        <v>741232.31429246697</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="B10">
-        <v>287417.48431020498</v>
+        <v>2296783.8983050799</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B11">
-        <v>199</v>
+        <v>287417.48431020498</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12">
-        <v>1314033.7881918801</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13">
-        <v>858888.40538922697</v>
+        <v>1314033.7881918801</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="B14">
-        <v>587333</v>
+        <v>858888.40538922697</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B15">
-        <v>2545.2924119999998</v>
+        <v>587333</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B16">
-        <v>4942.5355584795898</v>
+        <v>2545.2924119999998</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16">
       <c r="A17" s="1" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="B17">
-        <v>365365.4375</v>
+        <v>4942.5355584795898</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="B18">
-        <v>9715.0614771573091</v>
+        <v>365365.4375</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19">
-        <v>594</v>
+        <v>9715.0614771573091</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20">
-        <v>195.72</v>
+        <v>594</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="B21">
-        <v>618052.75086526002</v>
+        <v>195.72</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B22">
-        <v>2507.69425586742</v>
+        <v>618052.75086526002</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
-        <v>13386.72</v>
+        <v>2507.69425586742</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24">
-        <v>9643.7388078544791</v>
+        <v>13386.72</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16">
       <c r="A25" s="1" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
       <c r="B25">
-        <v>251658655.71277899</v>
+        <v>9643.7388078544791</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16">
       <c r="A26" s="1" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="B26">
-        <v>250935350.003824</v>
+        <v>246808065.925441</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <v>377260702.42225301</v>
+        <v>249890626.983358</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16">
       <c r="A28" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B28">
-        <v>135687530.408627</v>
+        <v>380308908.66714501</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>84195425.480663896</v>
+        <v>135687530.408627</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16">
       <c r="A30" s="1" t="s">
-        <v>159</v>
+        <v>33</v>
       </c>
       <c r="B30">
-        <v>7395659.7009212896</v>
+        <v>85644662.768799499</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>159</v>
       </c>
       <c r="B31">
-        <v>5202804.4875486996</v>
+        <v>7395659.7009212896</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32">
-        <v>14596149.849582899</v>
+        <v>5202804.4875486996</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16">
       <c r="A33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33">
-        <v>793333.33333333302</v>
+        <v>14596149.849582899</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34">
-        <v>100225</v>
+        <v>793333.33333333302</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35">
-        <v>8821748.2849042695</v>
+        <v>100225</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16">
       <c r="A36" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B36">
-        <v>40000</v>
+        <v>8821748.2849042695</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B37">
-        <v>9879467.9617414791</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16">
       <c r="A38" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="B38">
-        <v>282404665.385589</v>
+        <v>9879467.9617414791</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16">
       <c r="A39" s="1" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>267656871.20731199</v>
+        <v>282404665.385589</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16">
       <c r="A40" s="1" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="B40">
-        <v>244612695.44406801</v>
+        <v>267656871.20731199</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16">
       <c r="A41" s="1" t="s">
-        <v>156</v>
+        <v>6</v>
       </c>
       <c r="B41">
-        <v>265687203.37454599</v>
+        <v>244612695.44406801</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="B42">
-        <v>327951301.000947</v>
+        <v>265687203.37454599</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43">
-        <v>9315783.8983050808</v>
+        <v>327951301.000947</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16">
       <c r="A44" s="1" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="B44">
-        <v>47926596.969999999</v>
+        <v>9315783.8983050808</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="B45">
-        <v>56067143.149989001</v>
+        <v>47926596.969999999</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16">
       <c r="A46" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46">
-        <v>3000000</v>
+        <v>56067143.149989001</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16">
       <c r="A47" s="1" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="B47">
-        <v>1999.2794019999999</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16">
       <c r="A48" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B48">
-        <v>7789.1925490000003</v>
+        <v>1999.2794019999999</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16">
       <c r="A49" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49">
-        <v>86884.467919999996</v>
+        <v>7789.1925490000003</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16">
       <c r="A50" s="1" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="B50">
-        <v>366156088.48758399</v>
+        <v>86884.467919999996</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51">
-        <v>647123302.82240796</v>
+        <v>366156088.48758399</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16">
       <c r="A52" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B52">
-        <v>15154166.3333333</v>
+        <v>647123302.82240796</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16">
       <c r="A53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B53">
-        <v>4236515.3599999901</v>
+        <v>15154166.3333333</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16">
       <c r="A54" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B54">
-        <v>178126907.15206799</v>
+        <v>4236515.3599999901</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16">
       <c r="A55" s="1" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B55">
-        <v>27279530.952380899</v>
+        <v>178126907.15206799</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16">
       <c r="A56" s="1" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="B56">
-        <v>1999.2794019999999</v>
+        <v>27279530.952380899</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16">
       <c r="A57" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B57">
-        <v>321203.81650000002</v>
+        <v>1999.2794019999999</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="16">
       <c r="A58" s="1" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="B58">
-        <v>17705160.810299501</v>
+        <v>321203.81650000002</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="16">
       <c r="A59" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B59">
-        <v>262124830.59272301</v>
+        <v>17705160.810299501</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="16">
       <c r="A60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B60">
-        <v>262363802.82582599</v>
+        <v>262124830.59272301</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16">
       <c r="A61" s="1" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B61">
-        <v>512651919.961757</v>
+        <v>262363802.82582599</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="16">
       <c r="A62" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B62">
-        <v>327951301.000947</v>
+        <v>512651919.961757</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="16">
       <c r="A63" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B63">
-        <v>181196389.517434</v>
+        <v>327951301.000947</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16">
       <c r="A64" s="1" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
       <c r="B64">
-        <v>106339848.537673</v>
+        <v>181196389.517434</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="16">
       <c r="A65" s="1" t="s">
-        <v>11</v>
+        <v>157</v>
       </c>
       <c r="B65">
-        <v>315233432.18682897</v>
+        <v>106339848.537673</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="16">
       <c r="A66" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B66">
-        <v>531768.44999999995</v>
+        <v>315233432.18682897</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="16">
       <c r="A67" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67">
         <v>531768.44999999995</v>
@@ -1457,400 +1483,416 @@
     </row>
     <row r="68" spans="1:2" ht="16">
       <c r="A68" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B68">
-        <v>1643536.0106001699</v>
+        <v>531768.44999999995</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="16">
       <c r="A69" s="1" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="B69">
-        <v>266816.53177964699</v>
+        <v>1643536.0106001699</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="16">
       <c r="A70" s="1" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="B70">
-        <v>60587576.139797598</v>
+        <v>741232.31429246697</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="16">
       <c r="A71" s="1" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="B71">
-        <v>287417.48431020498</v>
+        <v>2296783.8983050799</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="16">
       <c r="A72" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B72">
-        <v>181</v>
+        <v>287417.48431020498</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="16">
       <c r="A73" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B73">
-        <v>923</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="16">
       <c r="A74" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B74">
-        <v>1226</v>
+        <v>923</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="16">
       <c r="A75" s="1" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="B75">
-        <v>633</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="16">
       <c r="A76" s="1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B76">
-        <v>222.92452080000001</v>
+        <v>633</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="16">
       <c r="A77" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B77">
-        <v>358.654464235619</v>
+        <v>222.92452080000001</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="16">
       <c r="A78" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B78">
-        <v>513.729031978796</v>
+        <v>358.654464235619</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="16">
       <c r="A79" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B79">
-        <v>845.19104734837197</v>
+        <v>513.729031978796</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="16">
       <c r="A80" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B80">
-        <v>594</v>
+        <v>845.19104734837197</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="16">
       <c r="A81" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B81">
-        <v>26</v>
+        <v>594</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="16">
       <c r="A82" s="1" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="B82">
-        <v>281</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="16">
       <c r="A83" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B83">
-        <v>923</v>
+        <v>281</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="16">
       <c r="A84" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B84">
-        <v>1226</v>
+        <v>923</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="16">
       <c r="A85" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B85">
-        <v>933</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="16">
       <c r="A86" s="1" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B86">
-        <v>578.09109640171903</v>
+        <v>933</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="16">
       <c r="A87" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B87">
-        <v>802.50077049713502</v>
+        <v>578.09109640171903</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="16">
       <c r="A88" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B88">
-        <v>231</v>
+        <v>802.50077049713502</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="16">
       <c r="A89" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B89">
-        <v>322.87188184190501</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="16">
       <c r="A90" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B90">
-        <v>245</v>
+        <v>322.87188184190501</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="16">
       <c r="A91" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B91">
-        <v>594</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="16">
       <c r="A92" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="B92">
-        <v>2453</v>
+        <v>594</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="16">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="B93">
-        <v>923</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="16">
       <c r="A94" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B94">
-        <v>1226</v>
+        <v>923</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="16">
       <c r="A95" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B95">
-        <v>933</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="16">
       <c r="A96" s="1" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="B96">
-        <v>199.11984128017099</v>
+        <v>933</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="16">
       <c r="A97" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B97">
-        <v>14.68</v>
+        <v>199.11984128017099</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="16">
       <c r="A98" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B98">
-        <v>94.78</v>
+        <v>14.68</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="16">
       <c r="A99" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B99">
-        <v>476.61081081081102</v>
+        <v>94.78</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="16">
       <c r="A100" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B100">
-        <v>7395659.7009212896</v>
+        <v>476.61081081081102</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="16">
       <c r="A101" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B101">
-        <v>4926635.1499049403</v>
+        <v>7395659.7009212896</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="16">
       <c r="A102" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B102">
-        <v>12767744.447830999</v>
+        <v>4926635.1499049403</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="16">
       <c r="A103" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B103">
-        <v>7395659.7009212896</v>
+        <v>12767744.447830999</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="16">
       <c r="A104" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B104">
-        <v>9991043.3145009391</v>
+        <v>7395659.7009212896</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="16">
       <c r="A105" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B105">
-        <v>18731502.137926701</v>
+        <v>9991043.3145009391</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="16">
       <c r="A106" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B106">
-        <v>33013074.907786202</v>
+        <v>18450727.8376109</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="16">
       <c r="A107" s="1" t="s">
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="B107">
-        <v>6447245.6891400497</v>
+        <v>511460.11998873699</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="16">
       <c r="A108" s="1" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="B108">
-        <v>7395659.7009212896</v>
+        <v>33618775.405666798</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="16">
       <c r="A109" s="1" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="B109">
-        <v>4478766.8760734303</v>
+        <v>31862130.341213599</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16">
       <c r="A110" s="1" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B110">
-        <v>7395659.7009212896</v>
+        <v>6429259.9306045799</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="16">
       <c r="A111" s="1" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="B111">
-        <v>250935350.003824</v>
+        <v>7395659.7009212896</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="16">
       <c r="A112" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B112">
-        <v>4926635.1499049403</v>
+        <v>4478766.8760734303</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="16">
       <c r="A113" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B113">
-        <v>669753.66372214095</v>
+        <v>7395659.7009212896</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="16">
       <c r="A114" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B114">
-        <v>369782.98504606402</v>
+        <v>4926635.1499049403</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="16">
       <c r="A115" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B115">
-        <v>518989.66055762197</v>
+        <v>669753.66372214095</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="16">
       <c r="A116" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B116">
+        <v>369782.98504606402</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="16">
+      <c r="A117" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B117">
+        <v>518989.66055762197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="16">
+      <c r="A118" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B116">
-        <v>209718.165600915</v>
+      <c r="B118">
+        <v>206347.75812919799</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B116">
-    <sortState ref="A2:B131">
-      <sortCondition ref="A1:A131"/>
+  <autoFilter ref="A1:B118">
+    <sortState ref="A2:B118">
+      <sortCondition ref="A1:A118"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1863,6 +1905,959 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B116"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="87.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>669753.66372214095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>369782.98504606402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>518989.66055762197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5">
+        <v>451954.62750842603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16">
+      <c r="A7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16">
+      <c r="A8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8">
+        <v>232359.57840255499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>62923335.085405901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16">
+      <c r="A10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16">
+      <c r="A11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16">
+      <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16">
+      <c r="A13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13">
+        <v>858888.40538922697</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>587333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <v>2545.2924119999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>4942.5355584795898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16">
+      <c r="A17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18">
+        <v>9715.0614771573091</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20">
+        <v>195.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21">
+        <v>618052.75086526002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>2507.69425586742</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16">
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>13386.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16">
+      <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <v>9643.7388078544791</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16">
+      <c r="A25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25">
+        <v>251658655.71277899</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>250935350.003824</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>377260702.42225301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>135687530.408627</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>84195425.480663896</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16">
+      <c r="A30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31">
+        <v>5202804.4875486996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32">
+        <v>14596149.849582899</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16">
+      <c r="A33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16">
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16">
+      <c r="A35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35">
+        <v>8821748.2849042695</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16">
+      <c r="A36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16">
+      <c r="A37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37">
+        <v>9879467.9617414791</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16">
+      <c r="A38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>282404665.385589</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="16">
+      <c r="A39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39">
+        <v>267656871.20731199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16">
+      <c r="A40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>244612695.44406801</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16">
+      <c r="A41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41">
+        <v>265687203.37454599</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16">
+      <c r="A42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42">
+        <v>327951301.000947</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43">
+        <v>9315783.8983050808</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16">
+      <c r="A44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16">
+      <c r="A45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45">
+        <v>56067143.149989001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16">
+      <c r="A46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="16">
+      <c r="A47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="16">
+      <c r="A48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="16">
+      <c r="A49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16">
+      <c r="A50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>366156088.48758399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16">
+      <c r="A51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>647123302.82240796</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16">
+      <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52">
+        <v>15154166.3333333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16">
+      <c r="A53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53">
+        <v>4236515.3599999901</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16">
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>178126907.15206799</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16">
+      <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55">
+        <v>27279530.952380899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16">
+      <c r="A56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16">
+      <c r="A57" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="16">
+      <c r="A58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58">
+        <v>17705160.810299501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16">
+      <c r="A59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>262124830.59272301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16">
+      <c r="A60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <v>262363802.82582599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16">
+      <c r="A61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61">
+        <v>512651919.961757</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="16">
+      <c r="A62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62">
+        <v>327951301.000947</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="16">
+      <c r="A63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>181196389.517434</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="16">
+      <c r="A64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64">
+        <v>106339848.537673</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="16">
+      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65">
+        <v>315233432.18682897</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="16">
+      <c r="A66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="16">
+      <c r="A67" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="16">
+      <c r="A68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="16">
+      <c r="A69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69">
+        <v>266816.53177964699</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="16">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>60587576.139797598</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="16">
+      <c r="A71" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="16">
+      <c r="A72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="16">
+      <c r="A73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="16">
+      <c r="A74" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="16">
+      <c r="A75" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="16">
+      <c r="A76" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76">
+        <v>222.92452080000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16">
+      <c r="A77" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77">
+        <v>358.654464235619</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="16">
+      <c r="A78" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B78">
+        <v>513.729031978796</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="16">
+      <c r="A79" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79">
+        <v>845.19104734837197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="16">
+      <c r="A80" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16">
+      <c r="A81" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B81">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16">
+      <c r="A82" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16">
+      <c r="A83" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16">
+      <c r="A84" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16">
+      <c r="A85" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="16">
+      <c r="A86" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86">
+        <v>578.09109640171903</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="16">
+      <c r="A87" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B87">
+        <v>802.50077049713502</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="16">
+      <c r="A88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16">
+      <c r="A89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89">
+        <v>322.87188184190501</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16">
+      <c r="A90" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="16">
+      <c r="A91" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16">
+      <c r="A92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="16">
+      <c r="A93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16">
+      <c r="A94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16">
+      <c r="A95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16">
+      <c r="A96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B96">
+        <v>199.11984128017099</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16">
+      <c r="A97" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B97">
+        <v>14.68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16">
+      <c r="A98" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B98">
+        <v>94.78</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16">
+      <c r="A99" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99">
+        <v>476.61081081081102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16">
+      <c r="A100" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B100">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16">
+      <c r="A101" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101">
+        <v>4926635.1499049403</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16">
+      <c r="A102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B102">
+        <v>12767744.447830999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16">
+      <c r="A103" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B103">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16">
+      <c r="A104" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B104">
+        <v>9991043.3145009391</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16">
+      <c r="A105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105">
+        <v>18731502.137926701</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16">
+      <c r="A106" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106">
+        <v>33013074.907786202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16">
+      <c r="A107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107">
+        <v>6447245.6891400497</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="16">
+      <c r="A108" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B108">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="16">
+      <c r="A109" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B109">
+        <v>4478766.8760734303</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="16">
+      <c r="A110" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B110">
+        <v>7395659.7009212896</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="16">
+      <c r="A111" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B111">
+        <v>250935350.003824</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="16">
+      <c r="A112" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112">
+        <v>4926635.1499049403</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="16">
+      <c r="A113" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B113">
+        <v>669753.66372214095</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="16">
+      <c r="A114" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114">
+        <v>369782.98504606402</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="16">
+      <c r="A115" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B115">
+        <v>518989.66055762197</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="16">
+      <c r="A116" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B116">
+        <v>209718.165600915</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
@@ -2940,12 +3935,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated cost specs to new dataset. Also added unit of euro.
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/total_costs.xlsx
+++ b/scripts/query_generator/cost_update/total_costs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="20130409" sheetId="4" r:id="rId1"/>
-    <sheet name="20121221" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="backup" sheetId="2" r:id="rId4"/>
+    <sheet name="20130904" sheetId="5" r:id="rId1"/>
+    <sheet name="20130409" sheetId="4" r:id="rId2"/>
+    <sheet name="20121221" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="backup" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'20121221'!$A$1:$B$116</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20130409'!$A$1:$B$118</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$B$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'20121221'!$A$1:$B$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'20130409'!$A$1:$B$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$B$131</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="177">
   <si>
     <t>key</t>
   </si>
@@ -519,6 +520,45 @@
   </si>
   <si>
     <t>industry_chp_turbine_gas_power_fuelmix</t>
+  </si>
+  <si>
+    <t>energy_power_ultra_supercritical_cofiring_coal</t>
+  </si>
+  <si>
+    <t>energy_chp_ultra_supercritical_cofiring_coal</t>
+  </si>
+  <si>
+    <t>buildings_collective_chp_network_gas</t>
+  </si>
+  <si>
+    <t>agriculture_chp_supercritical_wood_pellets</t>
+  </si>
+  <si>
+    <t>energy_chp_supercritical_waste_mix</t>
+  </si>
+  <si>
+    <t>other_chp_engine_biogas</t>
+  </si>
+  <si>
+    <t>buildings_chp_engine_biogas</t>
+  </si>
+  <si>
+    <t>households_collective_chp_biogas</t>
+  </si>
+  <si>
+    <t>industry_steel_electricfurnace_burner_network_gas</t>
+  </si>
+  <si>
+    <t>industry_aluminium_burner_network_gas</t>
+  </si>
+  <si>
+    <t>industry_steel_blastfurnace_burner_coal_gas</t>
+  </si>
+  <si>
+    <t>industry_other_metals_burner_network_gas</t>
+  </si>
+  <si>
+    <t>buildings_cooling_airconditioning_electricity</t>
   </si>
 </sst>
 </file>
@@ -572,8 +612,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -591,19 +643,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -933,9 +997,1302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B168"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>242820426.756551</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>260609607.419949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>230600996.20282301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>167937238.66356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>179931584.889873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>315047016.93954301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>176157457.43679699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>7187319.3052229797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9">
+        <v>344201361.34674698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10">
+        <v>358349929.07627702</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>260840943.60714999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>281120213.17249697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>330064895.03167301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14">
+        <v>684410.00703404297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15">
+        <v>57135195.933596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <v>260295067.11974001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>67549434.658698097</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18">
+        <v>535713.76296021498</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19">
+        <v>33166602.271356098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20">
+        <v>263181591.906753</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21">
+        <v>104285238.659437</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>17417062.278448299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23">
+        <v>752461.25791329797</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24">
+        <v>728323.800905757</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27">
+        <v>728323.800905757</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>366049307.44920897</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>621955451.00600398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34">
+        <v>2920458.2203389802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35">
+        <v>2280121.0593220298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>2280121.0593220298</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37">
+        <v>698724.90954199096</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>4236515.76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>15154166.666666601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41">
+        <v>16035000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>56067143.149989001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44">
+        <v>330064895.03167301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>27648900</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46">
+        <v>638724.90954199096</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47">
+        <v>638724.90954199096</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48">
+        <v>2545.2924119999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49">
+        <v>638724.90954199096</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50">
+        <v>222.92452080000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51">
+        <v>675607.926374426</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52">
+        <v>361379.298158472</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53">
+        <v>529205.73744889896</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54">
+        <v>7227585.9631694397</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55">
+        <v>12878997.9797897</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56">
+        <v>4896284.18237634</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57">
+        <v>10185359.416195801</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>172</v>
+      </c>
+      <c r="B58">
+        <v>7227585.9631694397</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59">
+        <v>7227585.9631694397</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60">
+        <v>4404521.3721229602</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61">
+        <v>6127282.2065939596</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62">
+        <v>361379.298158472</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63">
+        <v>4896284.18237634</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64">
+        <v>675607.926374426</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65">
+        <v>529205.73744889896</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66">
+        <v>2452.3561710138301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67">
+        <v>9784.8378954938798</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>49</v>
+      </c>
+      <c r="B68">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69">
+        <v>587333.33333333302</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>54</v>
+      </c>
+      <c r="B71">
+        <v>9764.2489147085507</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B72">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73">
+        <v>4923.6543012899201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76">
+        <v>476.61081081081102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78">
+        <v>321.01370887396899</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80">
+        <v>196.89045470632701</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>327.452895613245</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>61</v>
+      </c>
+      <c r="B83">
+        <v>721.01685704343595</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86">
+        <v>708.36500733229104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>66</v>
+      </c>
+      <c r="B87">
+        <v>633.33333333333303</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91">
+        <v>8617334.2795304004</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>10070912.396908799</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93">
+        <v>14724400.448924299</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94">
+        <v>5169081.1902946997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>159</v>
+      </c>
+      <c r="B95">
+        <v>7227585.9631694397</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>60</v>
+      </c>
+      <c r="B96">
+        <v>481.74203221112703</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>56</v>
+      </c>
+      <c r="B97">
+        <v>440.98996479434697</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>92</v>
+      </c>
+      <c r="B98">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+      <c r="B100">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102">
+        <v>614647.124820053</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>176</v>
+      </c>
+      <c r="B103">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104">
+        <v>851570.08750594</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>94</v>
+      </c>
+      <c r="B105">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>99</v>
+      </c>
+      <c r="B109">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>100</v>
+      </c>
+      <c r="B110">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>103</v>
+      </c>
+      <c r="B111">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>105</v>
+      </c>
+      <c r="B113">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>104</v>
+      </c>
+      <c r="B114">
+        <v>281.666666666666</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>160</v>
+      </c>
+      <c r="B115">
+        <v>698724.90954199096</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>167</v>
+      </c>
+      <c r="B116">
+        <v>2920458.2203389802</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>161</v>
+      </c>
+      <c r="B117">
+        <v>684410.00703404297</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>260609607.419949</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119">
+        <v>167937238.66356</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>154</v>
+      </c>
+      <c r="B120">
+        <v>57135195.933596</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>12</v>
+      </c>
+      <c r="B121">
+        <v>67549434.658698097</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>162</v>
+      </c>
+      <c r="B122">
+        <v>535713.76296021498</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>163</v>
+      </c>
+      <c r="B123">
+        <v>33166602.271356098</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124">
+        <v>7187319.3052229797</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>168</v>
+      </c>
+      <c r="B125">
+        <v>16035000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>165</v>
+      </c>
+      <c r="B126">
+        <v>358349929.07627702</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>158</v>
+      </c>
+      <c r="B127">
+        <v>752461.25791329797</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>169</v>
+      </c>
+      <c r="B128">
+        <v>638724.90954199096</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>166</v>
+      </c>
+      <c r="B129">
+        <v>728323.800905757</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>29</v>
+      </c>
+      <c r="B130">
+        <v>2280121.0593220298</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>170</v>
+      </c>
+      <c r="B131">
+        <v>638724.90954199096</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>110</v>
+      </c>
+      <c r="B132">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>109</v>
+      </c>
+      <c r="B134">
+        <v>728323.800905757</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>108</v>
+      </c>
+      <c r="B135">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>30</v>
+      </c>
+      <c r="B136">
+        <v>2280121.0593220298</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>171</v>
+      </c>
+      <c r="B137">
+        <v>638724.90954199096</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>124</v>
+      </c>
+      <c r="B160">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>125</v>
+      </c>
+      <c r="B161">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>135</v>
+      </c>
+      <c r="B162">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>136</v>
+      </c>
+      <c r="B163">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>137</v>
+      </c>
+      <c r="B164">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>138</v>
+      </c>
+      <c r="B165">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1904,7 +3261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
@@ -2857,7 +4214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
@@ -3935,12 +5292,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:G6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated cost specs to reflect the changes as a result of moving to 2012 data.
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/total_costs.xlsx
+++ b/scripts/query_generator/cost_update/total_costs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21880" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16020" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="20131125" sheetId="7" r:id="rId1"/>
@@ -15,13 +15,16 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
     <sheet name="backup" sheetId="2" r:id="rId7"/>
     <sheet name="20140702" sheetId="8" r:id="rId8"/>
+    <sheet name="20140725" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20121221'!$A$1:$B$116</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'20130409'!$A$1:$B$118</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'20131125'!$A$1:$B$125</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'20140702'!$A$1:$B$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'20140725'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$A$1:$B$131</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="8">'20140725'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="183">
   <si>
     <t>key</t>
   </si>
@@ -635,8 +638,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -694,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -721,6 +756,22 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -747,6 +798,22 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4790,8 +4857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5743,7 +5810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A108" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -6821,9 +6888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -8068,14 +8133,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -9240,6 +9306,1026 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>755051.04850575002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>331312.397213977</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>523510.37098146603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5">
+        <v>701158.87573600002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6">
+        <v>598514.16246077802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7">
+        <v>2603019.54717266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10">
+        <v>641158.87573600002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11">
+        <v>625460.18051197496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>2579919.54717266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16">
+        <v>825386.444324043</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>587333.33333333302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>2545.2924119999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>4597.5249502164097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <v>10722.666409257899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24">
+        <v>602462.398958073</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25">
+        <v>2253.1737123554499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27">
+        <v>9697.0656672772893</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28">
+        <v>44267272.9061542</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29">
+        <v>19245000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>190819641.20650199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31">
+        <v>280584476.09997702</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>199982710.29333299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33">
+        <v>6669208.39075734</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34">
+        <v>4686963.2744296798</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>16538315.3132316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38">
+        <v>7938226.4211913599</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40">
+        <v>9964183.9307831004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>235374124.11816999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42">
+        <v>130767381.291293</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>215524754.77994499</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44">
+        <v>120058747.125983</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45">
+        <v>1038793.0315475099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46">
+        <v>2444820.02873547</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49">
+        <v>56752467.806564301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54">
+        <v>382137001.128667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55">
+        <v>614878773.55227995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56">
+        <v>15172516.666666601</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57">
+        <v>4236515.76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58">
+        <v>209495043.47684801</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59">
+        <v>27436675</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62">
+        <v>8846298.7691968605</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63">
+        <v>269820764.13113302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64">
+        <v>217266313.53025201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65">
+        <v>370724043.04133999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66">
+        <v>371680319.98421502</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>181265194.89712</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>157</v>
+      </c>
+      <c r="B68">
+        <v>83892075.861641705</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>316715428.23878002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73">
+        <v>641158.87573600002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74">
+        <v>625460.18051197496</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75">
+        <v>2579919.54717266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80">
+        <v>633.33333333333303</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81">
+        <v>222.92452080000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>316.73240840377798</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83">
+        <v>445.17235548857201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84">
+        <v>831.37481336900805</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>59</v>
+      </c>
+      <c r="B86">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>104</v>
+      </c>
+      <c r="B87">
+        <v>281.666666666666</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>102</v>
+      </c>
+      <c r="B88">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>108</v>
+      </c>
+      <c r="B90">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91">
+        <v>487.32029579955002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92">
+        <v>753.41144995645004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>62</v>
+      </c>
+      <c r="B93">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>63</v>
+      </c>
+      <c r="B94">
+        <v>301.25496704147997</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>64</v>
+      </c>
+      <c r="B95">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>17</v>
+      </c>
+      <c r="B97">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>110</v>
+      </c>
+      <c r="B100">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>67</v>
+      </c>
+      <c r="B101">
+        <v>170.348861199998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>68</v>
+      </c>
+      <c r="B102">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>69</v>
+      </c>
+      <c r="B103">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104">
+        <v>476.61081081081102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>173</v>
+      </c>
+      <c r="B105">
+        <v>6669208.39075734</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>75</v>
+      </c>
+      <c r="B106">
+        <v>4462378.0580978198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>76</v>
+      </c>
+      <c r="B107">
+        <v>14452514.4885864</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>77</v>
+      </c>
+      <c r="B108">
+        <v>6669208.39075734</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>78</v>
+      </c>
+      <c r="B109">
+        <v>10077030.023078101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>181</v>
+      </c>
+      <c r="B110">
+        <v>4462378.0580978198</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>182</v>
+      </c>
+      <c r="B111">
+        <v>14452514.4885864</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>180</v>
+      </c>
+      <c r="B112">
+        <v>6669208.39075734</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>179</v>
+      </c>
+      <c r="B113">
+        <v>10077030.023078101</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114">
+        <v>52363330.154113002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>162</v>
+      </c>
+      <c r="B115">
+        <v>516377.85671238002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>163</v>
+      </c>
+      <c r="B116">
+        <v>24927067.4977035</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117">
+        <v>6481810.7618950102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>175</v>
+      </c>
+      <c r="B118">
+        <v>4576654.6459953701</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>174</v>
+      </c>
+      <c r="B119">
+        <v>3818439.7286856002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>172</v>
+      </c>
+      <c r="B120">
+        <v>6669208.39075734</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>79</v>
+      </c>
+      <c r="B121">
+        <v>4462378.0580978198</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>80</v>
+      </c>
+      <c r="B122">
+        <v>755051.04850575002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>81</v>
+      </c>
+      <c r="B123">
+        <v>331312.397213977</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>82</v>
+      </c>
+      <c r="B124">
+        <v>523510.37098146603</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B172">
+    <sortCondition ref="A2:A172"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fixes issue #72 (cost update)
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/total_costs.xlsx
+++ b/scripts/query_generator/cost_update/total_costs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="22440" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="22440" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="20131125" sheetId="7" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="20140702" sheetId="8" r:id="rId8"/>
     <sheet name="20140725" sheetId="9" r:id="rId9"/>
     <sheet name="Blad1" sheetId="10" r:id="rId10"/>
+    <sheet name="20150812" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20121221'!$A$1:$B$116</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="186">
   <si>
     <t>key</t>
   </si>
@@ -593,6 +594,9 @@
   </si>
   <si>
     <t>new query:</t>
+  </si>
+  <si>
+    <t>households_flexibility_p2h_electricity</t>
   </si>
 </sst>
 </file>
@@ -742,50 +746,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="89">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -830,7 +834,7 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -3173,6 +3177,998 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B121"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1">
+        <v>2569593.9226519298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2">
+        <v>560427.79114020802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3">
+        <v>1673650.70153317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>1716.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>2569593.9226519298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9">
+        <v>1673650.70153317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <v>560427.79114020802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>193.44800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12">
+        <v>539985.01202618703</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13">
+        <v>2592693.9226519298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14">
+        <v>1733650.70153317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>8541708.4726709593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>238164513.43279701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>389752235.32731402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>27436675</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20">
+        <v>123664833.60449199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>2549275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>15172516.666666601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23">
+        <v>39828957.156776898</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>621647870.61774302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>56752467.806564301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27">
+        <v>279556398.64126098</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>201099715.413333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29">
+        <v>19245000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>216809177.16655901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31">
+        <v>112004025.951187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32">
+        <v>76297624.468262807</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>208962682.14191401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>234701099.40801799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>215277964.757128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>316870089.761751</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>182275127.09775999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39">
+        <v>26338023.342601601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40">
+        <v>368919195.94714898</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>268558508.11190999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44">
+        <v>1184627.8934179901</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45">
+        <v>20646248.698130101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>43756392.885129496</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47">
+        <v>429654.69828056003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>5751049.72976973</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>190559247.075284</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>4579.09575498505</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>9658.1098226707909</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54">
+        <v>585227.57368030504</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59">
+        <v>1971.43779869941</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60">
+        <v>587333.33333333302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61">
+        <v>788350.68984855502</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62">
+        <v>7199.8736234659</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>176</v>
+      </c>
+      <c r="B63">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64">
+        <v>4453269.6883829301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65">
+        <v>5829216.03967149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66">
+        <v>8797195.1222331394</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67">
+        <v>10014215.807243699</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68">
+        <v>5829216.03967149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69">
+        <v>4116764.7597511001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70">
+        <v>5829216.03967149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71">
+        <v>4453269.6883829301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72">
+        <v>10014215.807243699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>182</v>
+      </c>
+      <c r="B73">
+        <v>8797195.1222331394</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74">
+        <v>5829216.03967149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75">
+        <v>3918308.7589525301</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80">
+        <v>155.98320045211</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83">
+        <v>290.56053070694099</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>65</v>
+      </c>
+      <c r="B86">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B88">
+        <v>750.70330712372095</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90">
+        <v>281.666666666666</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91">
+        <v>445.03398511053302</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>55</v>
+      </c>
+      <c r="B93">
+        <v>315.44598104960198</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>56</v>
+      </c>
+      <c r="B94">
+        <v>413.46753022970302</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>58</v>
+      </c>
+      <c r="B95">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>57</v>
+      </c>
+      <c r="B97">
+        <v>586.66114406867996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98">
+        <v>633.33333333333303</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99">
+        <v>4453269.6883829301</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>82</v>
+      </c>
+      <c r="B100">
+        <v>520207.943373908</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101">
+        <v>456636.51597914402</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>81</v>
+      </c>
+      <c r="B102">
+        <v>288783.92424773198</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103">
+        <v>288783.92424773198</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>91</v>
+      </c>
+      <c r="B104">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>92</v>
+      </c>
+      <c r="B105">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106">
+        <v>520207.943373908</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107">
+        <v>456636.51597914402</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>84</v>
+      </c>
+      <c r="B108">
+        <v>4676842.8636353603</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109">
+        <v>6916614.1023031604</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>159</v>
+      </c>
+      <c r="B111">
+        <v>5829216.03967149</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>90</v>
+      </c>
+      <c r="B112">
+        <v>9902298.0038525797</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>89</v>
+      </c>
+      <c r="B113">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>86</v>
+      </c>
+      <c r="B114">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>85</v>
+      </c>
+      <c r="B115">
+        <v>10018988.821463199</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>136</v>
+      </c>
+      <c r="B119">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>137</v>
+      </c>
+      <c r="B120">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>138</v>
+      </c>
+      <c r="B121">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
@@ -10336,8 +11332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated cost specs to reflect changes describes in quintel/etsource#935
</commit_message>
<xml_diff>
--- a/scripts/query_generator/cost_update/total_costs.xlsx
+++ b/scripts/query_generator/cost_update/total_costs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="22440" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16140" tabRatio="500" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="20131125" sheetId="7" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="20140725" sheetId="9" r:id="rId9"/>
     <sheet name="Blad1" sheetId="10" r:id="rId10"/>
     <sheet name="20150812" sheetId="11" r:id="rId11"/>
+    <sheet name="20150817" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'20121221'!$A$1:$B$116</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="186">
   <si>
     <t>key</t>
   </si>
@@ -650,8 +651,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -745,7 +754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -790,6 +799,10 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -834,6 +847,10 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3181,8 +3198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B121"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4161,6 +4178,999 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1">
+        <v>2723593.9226519298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2">
+        <v>567345.39723509096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>1716.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>2453.3333333333298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <v>933.33333333333303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>2723593.9226519298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <v>567345.39723509096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>193.44800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12">
+        <v>522910.85751158203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13">
+        <v>2615893.9226519298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14">
+        <v>1691150.70153317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>8542711.8949343897</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>1643536.0106001699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>238299117.49039701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>389752235.32731402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>27436675</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20">
+        <v>123660642.97733299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>2549275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>15172516.666666601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23">
+        <v>39843578.452615403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>621647870.61774302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>56752467.806564301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27">
+        <v>279660189.01210499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>201505203.573333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29">
+        <v>19245000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>217173596.69085401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31">
+        <v>112030560.895487</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32">
+        <v>76322643.130030796</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>209387069.43603101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>15969915.2575</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>234729173.82218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>215474700.58883801</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>316926234.01324099</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>182641746.32128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39">
+        <v>26338032.819367401</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40">
+        <v>369101405.709297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>531768.44999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>268611161.59955698</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44">
+        <v>1106589.20173967</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45">
+        <v>20655369.5223893</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>44184731.0503067</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47">
+        <v>429600.48393909598</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>5761794.4890970401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>190766827.816971</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50">
+        <v>1314033.7881918801</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>4579.09575498505</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>9658.1098226707909</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54">
+        <v>585205.73772175598</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>13387.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56">
+        <v>195.75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58">
+        <v>365365.4375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59">
+        <v>1971.0808485340899</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60">
+        <v>587333.33333333302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61">
+        <v>788303.766761926</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62">
+        <v>7199.8736234659</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>176</v>
+      </c>
+      <c r="B63">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64">
+        <v>4460530.6897432096</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65">
+        <v>5831983.2552912803</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66">
+        <v>8802896.5365704894</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>179</v>
+      </c>
+      <c r="B67">
+        <v>10014215.807243699</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68">
+        <v>5831983.2552912803</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69">
+        <v>4121561.66890524</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70">
+        <v>5831983.2552912803</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71">
+        <v>4460530.6897432096</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72">
+        <v>10014215.807243699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>182</v>
+      </c>
+      <c r="B73">
+        <v>8802896.5365704894</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74">
+        <v>5831983.2552912803</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75">
+        <v>3923656.88004041</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80">
+        <v>155.96499963094899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83">
+        <v>290.546981206743</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85">
+        <v>95.55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>65</v>
+      </c>
+      <c r="B86">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87">
+        <v>923.33333333333303</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B88">
+        <v>750.70330712372095</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90">
+        <v>281.666666666666</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91">
+        <v>444.98040974133102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92">
+        <v>1226.6666666666599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>55</v>
+      </c>
+      <c r="B93">
+        <v>315.44598104960198</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>56</v>
+      </c>
+      <c r="B94">
+        <v>413.427361255606</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>58</v>
+      </c>
+      <c r="B95">
+        <v>594.33333333333303</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96">
+        <v>287417.48431020498</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>57</v>
+      </c>
+      <c r="B97">
+        <v>586.66114406867996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98">
+        <v>633.33333333333303</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99">
+        <v>4460530.6897432096</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>82</v>
+      </c>
+      <c r="B100">
+        <v>520207.943373908</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101">
+        <v>456636.51597914402</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>81</v>
+      </c>
+      <c r="B102">
+        <v>288730.04206686502</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103">
+        <v>288730.04206686502</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>91</v>
+      </c>
+      <c r="B104">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>92</v>
+      </c>
+      <c r="B105">
+        <v>404644.32235354203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106">
+        <v>520207.943373908</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107">
+        <v>456636.51597914402</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>84</v>
+      </c>
+      <c r="B108">
+        <v>4684910.64292455</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109">
+        <v>6919979.6348137204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110">
+        <v>100225</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>159</v>
+      </c>
+      <c r="B111">
+        <v>5831983.2552912803</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>90</v>
+      </c>
+      <c r="B112">
+        <v>9902298.0038525797</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>89</v>
+      </c>
+      <c r="B113">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>86</v>
+      </c>
+      <c r="B114">
+        <v>793333.33333333302</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>85</v>
+      </c>
+      <c r="B115">
+        <v>10025561.2852132</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>124</v>
+      </c>
+      <c r="B116">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117">
+        <v>1999.2794019999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118">
+        <v>7789.1925490000003</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>136</v>
+      </c>
+      <c r="B119">
+        <v>86884.467919999996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>137</v>
+      </c>
+      <c r="B120">
+        <v>321203.81650000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>138</v>
+      </c>
+      <c r="B121">
+        <v>47926596.969999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7815,7 +8825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>